<commit_message>
Projektplan weitergeführt, Zeiterfassung erstellt
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\svm-c113.hsr.ch\pbuetiko\Documents\GitHub\Semesterarbeit-HS-2017-2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Documents\GitHub\Semesterarbeit-HS-2017-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,38 +24,82 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>ToDo-List</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Offene Fragen</t>
   </si>
   <si>
     <t>Werden uns reale Daten zum Vergleich mit unseren Simulationen zur Verfügung gestellt?</t>
   </si>
+  <si>
+    <t>ToDo-Liste</t>
+  </si>
+  <si>
+    <t>Wer</t>
+  </si>
+  <si>
+    <t>Termin</t>
+  </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>Erledigt</t>
+  </si>
+  <si>
+    <t>Frage</t>
+  </si>
+  <si>
+    <t>Lösung</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -63,12 +107,99 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -348,31 +479,372 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A49" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:I54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+    </row>
+    <row r="57" spans="1:9" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5"/>
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+      <c r="F65" s="5"/>
+      <c r="G65" s="5"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="A62:E62"/>
+    <mergeCell ref="F62:I62"/>
+    <mergeCell ref="A53:I54"/>
+    <mergeCell ref="A56:E56"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="A57:E57"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="A60:E60"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="F65:I65"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;G&amp;CEntwicklung einer Klassenbibliothek zur
+Erzeugung autokorrelierter Zufallszahlen&amp;R&amp;D</oddHeader>
+    <oddFooter>&amp;L&amp;P&amp;R&amp;F</oddFooter>
+  </headerFooter>
+  <legacyDrawingHF r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Zeiterfassung & ToDO-Liste geführt
</commit_message>
<xml_diff>
--- a/ToDoList.xlsx
+++ b/ToDoList.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\svm-c113.hsr.ch\adelay\Documents\SemesterArbeit\Semesterarbeit-HS-2017-2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Philipp\Documents\GitHub\Semesterarbeit-HS-2017-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>Offene Fragen</t>
   </si>
@@ -75,12 +75,39 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Simio-Temlate für .Net analysieren</t>
+  </si>
+  <si>
+    <t>Dokumentation: Autokorrelation TODOs ergänzen</t>
+  </si>
+  <si>
+    <t>MatNet.Numerics analysieren; Klassen identifizieren die gebraucht werden</t>
+  </si>
+  <si>
+    <t>Simio-Aktivierung über KMS abschliessen</t>
+  </si>
+  <si>
+    <t>Regression, Varianz und Kovarianz untersuchen und dokmentieren</t>
+  </si>
+  <si>
+    <t>.Net Core-Kompatibilität bestätigen (mit Mathnet.Numerics)</t>
+  </si>
+  <si>
+    <t>Statistische Tests definieren (Durbin Watson Test?)</t>
+  </si>
+  <si>
+    <t>SAD: Factory-Methoden dokumentieren</t>
+  </si>
+  <si>
+    <t>SAD: MathNet.Numerics dokumentieren</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,18 +214,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -206,6 +235,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -218,26 +253,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -518,21 +538,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="8.75" style="1"/>
-    <col min="8" max="8" width="9.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.75" style="1"/>
+    <col min="1" max="7" width="8.69921875" style="1"/>
+    <col min="8" max="8" width="9.8984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
@@ -545,7 +565,7 @@
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -556,199 +576,348 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="3" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:9" ht="29.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="4" t="s">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="3">
         <v>43012</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="4" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="3">
         <v>43013</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="4" t="s">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="3">
         <v>43014</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="I7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="4" t="s">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="3">
         <v>43015</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I8" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="4" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="3">
         <v>43016</v>
       </c>
-      <c r="I9" s="18" t="s">
+      <c r="I9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="4" t="s">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="3">
         <v>43017</v>
       </c>
-      <c r="I10" s="18" t="s">
+      <c r="I10" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="16"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="16"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="16"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I15" s="17"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I16" s="17"/>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I17" s="17"/>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I18" s="17"/>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I19" s="17"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="3">
+        <v>43040</v>
+      </c>
+      <c r="I11" s="15"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="3">
+        <v>43040</v>
+      </c>
+      <c r="I12" s="15"/>
+    </row>
+    <row r="13" spans="1:9" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="3">
+        <v>43047</v>
+      </c>
+      <c r="I13" s="15"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="3">
+        <v>43033</v>
+      </c>
+      <c r="I14" s="15"/>
+    </row>
+    <row r="15" spans="1:9" ht="26.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="3">
+        <v>43047</v>
+      </c>
+      <c r="I15" s="15"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="3">
+        <v>43040</v>
+      </c>
+      <c r="I16" s="15"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="3">
+        <v>43047</v>
+      </c>
+      <c r="I17" s="15"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="15"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="15"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="15"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="15"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="15"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="15"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="15"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>0</v>
       </c>
@@ -761,7 +930,7 @@
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -772,35 +941,35 @@
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8" t="s">
+      <c r="B56" s="10"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="10"/>
+      <c r="F56" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-    </row>
-    <row r="57" spans="1:9" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="9" t="s">
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+    </row>
+    <row r="57" spans="1:9" ht="32.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="10"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="6"/>
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
@@ -811,7 +980,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="6"/>
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
@@ -822,7 +991,7 @@
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="6"/>
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
@@ -833,7 +1002,7 @@
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="6"/>
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
@@ -844,7 +1013,7 @@
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="6"/>
       <c r="B62" s="6"/>
       <c r="C62" s="6"/>
@@ -855,7 +1024,7 @@
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="6"/>
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
@@ -866,7 +1035,7 @@
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="6"/>
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
@@ -877,7 +1046,7 @@
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="6"/>
       <c r="B65" s="6"/>
       <c r="C65" s="6"/>
@@ -888,7 +1057,7 @@
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="6"/>
       <c r="B66" s="6"/>
       <c r="C66" s="6"/>
@@ -900,19 +1069,27 @@
       <c r="I66" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="A14:F14"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
+  <mergeCells count="47">
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A20:F20"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A18:F18"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A66:E66"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="A63:E63"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="A64:E64"/>
+    <mergeCell ref="F64:I64"/>
+    <mergeCell ref="A65:E65"/>
+    <mergeCell ref="F65:I65"/>
     <mergeCell ref="A61:E61"/>
     <mergeCell ref="F61:I61"/>
     <mergeCell ref="A62:E62"/>
@@ -928,14 +1105,18 @@
     <mergeCell ref="F59:I59"/>
     <mergeCell ref="A60:E60"/>
     <mergeCell ref="F60:I60"/>
-    <mergeCell ref="A66:E66"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="A63:E63"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="A64:E64"/>
-    <mergeCell ref="F64:I64"/>
-    <mergeCell ref="A65:E65"/>
-    <mergeCell ref="F65:I65"/>
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>